<commit_message>
sua file_code chay dung_testok
</commit_message>
<xml_diff>
--- a/abc.xlsx
+++ b/abc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>target</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>thoat</t>
-  </si>
-  <si>
-    <t>nguyentuananh2019</t>
   </si>
 </sst>
 </file>
@@ -488,7 +485,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>19</v>

</xml_diff>